<commit_message>
Optimization and changed logic for get info about vulnerable components and gen graph
</commit_message>
<xml_diff>
--- a/reports/draft.xlsx
+++ b/reports/draft.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddpavlov\Desktop\Личная папка\Scripts\Dependency Track\dt-report-generator\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denimoll/Files/Programming shits/dt-report-generator/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61894AD1-7AE7-4205-90CA-68A9C48D1A27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A74A001-0871-304B-89E2-A5E39221240C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General information" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Vulnerable dependencies" sheetId="2" r:id="rId2"/>
     <sheet name="All issues" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>№</t>
   </si>
@@ -51,20 +51,35 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Recommended version</t>
-  </si>
-  <si>
-    <t>Vulnerability ID</t>
+    <t>Count of vulnerable dependencies</t>
+  </si>
+  <si>
+    <t>Last version</t>
+  </si>
+  <si>
+    <t>Final severity</t>
+  </si>
+  <si>
+    <t>Vulnerability</t>
   </si>
   <si>
     <t>Severity</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Verison</t>
+  </si>
+  <si>
+    <t>Report generated by dt-report-generator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +96,21 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -178,11 +208,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -205,8 +251,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -217,6 +267,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -255,29 +315,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A1:E9999" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:E9999" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблица1" displayName="Таблица1" ref="A1:F9999" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F9999" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Dependency"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Used version" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Group"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Recommended version" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{285D99C5-8A98-2543-AEE5-A809E9291686}" name="Final severity"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Last version" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Таблица2" displayName="Таблица2" ref="A1:F9999" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:F9999" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="№" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Dependency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Used version" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Group"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Vulnerability ID"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Severity"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB748631-99CD-E64B-B79C-4310C8831AA6}" name="Таблица13" displayName="Таблица13" ref="A1:E9999" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:E9999" xr:uid="{AA918DB4-2484-7040-BD07-7776E141CE3F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1C7933C9-3C85-7448-9754-6292512DCAFC}" name="№" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C83DC10C-1585-F04B-ADC5-44A9BA98F3D9}" name="Vulnerability"/>
+    <tableColumn id="3" xr3:uid="{FFC137A4-FB67-3D45-88EB-DD55BF6795F0}" name="Severity" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{1A434919-AB14-964F-9CA9-DD4331C139F6}" name="Component"/>
+    <tableColumn id="6" xr3:uid="{E8635739-AAAF-CA48-B42D-D80511409E7A}" name="Verison"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -568,74 +628,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5546875" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="2:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="8"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:D9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B9:D9" r:id="rId1" display="Report generated by dt-report-generator" xr:uid="{CCFE3F07-D623-804F-82CB-1792C41C87B9}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +729,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -662,41 +745,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{497817E8-1089-EF44-AD2C-86D494CB5712}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" style="2" customWidth="1"/>
-    <col min="4" max="6" width="25.6640625" customWidth="1"/>
+    <col min="4" max="5" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>11</v>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>